<commit_message>
clean up and make sure things work
</commit_message>
<xml_diff>
--- a/Atka mackerel/Data/atka_single_species_2022.xlsx
+++ b/Atka mackerel/Data/atka_single_species_2022.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20412"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20416"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\grant.adams\GitHub\RceattleRuns\Atka mackerel\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\grant.adams\GitHub\Rceattle-models\Atka mackerel\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B46394D2-0778-4706-BD70-8CCE3F803E53}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB2BE1F0-B0A0-436C-9D81-AEC17B2F3B5C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="495" windowWidth="19170" windowHeight="5115" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="495" windowWidth="19170" windowHeight="5115" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="meta_data" sheetId="1" r:id="rId1"/>
     <sheet name="control" sheetId="2" r:id="rId2"/>
     <sheet name="fleet_control" sheetId="3" r:id="rId3"/>
-    <sheet name="srv_biom" sheetId="4" r:id="rId4"/>
-    <sheet name="fsh_biom" sheetId="5" r:id="rId5"/>
+    <sheet name="index_data" sheetId="4" r:id="rId4"/>
+    <sheet name="catch_data" sheetId="5" r:id="rId5"/>
     <sheet name="comp_data" sheetId="6" r:id="rId6"/>
     <sheet name="emp_sel" sheetId="7" r:id="rId7"/>
     <sheet name="NByageFixed" sheetId="8" r:id="rId8"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="817" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="817" uniqueCount="271">
   <si>
     <t>Number</t>
   </si>
@@ -374,12 +374,6 @@
     <t>Age_first_selected</t>
   </si>
   <si>
-    <t>Accumatation_age_lower</t>
-  </si>
-  <si>
-    <t>Accumatation_age_upper</t>
-  </si>
-  <si>
     <t>Weight1_Numbers2</t>
   </si>
   <si>
@@ -852,6 +846,18 @@
   </si>
   <si>
     <t>Atka mackerel</t>
+  </si>
+  <si>
+    <t>Age_max_selected</t>
+  </si>
+  <si>
+    <t>Comp_loglike</t>
+  </si>
+  <si>
+    <t>Estimate_index_sd</t>
+  </si>
+  <si>
+    <t>Index_sd_prior</t>
   </si>
 </sst>
 </file>
@@ -1289,10 +1295,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>1</v>
@@ -1301,7 +1307,7 @@
         <v>2</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -1309,7 +1315,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
@@ -1318,13 +1324,13 @@
         <v>4</v>
       </c>
       <c r="E2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="F2" t="s">
         <v>105</v>
       </c>
       <c r="G2" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -1332,7 +1338,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C3" t="s">
         <v>5</v>
@@ -1341,13 +1347,13 @@
         <v>6</v>
       </c>
       <c r="E3" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="F3" t="s">
         <v>106</v>
       </c>
       <c r="G3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1355,7 +1361,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C4" t="s">
         <v>7</v>
@@ -1364,13 +1370,13 @@
         <v>8</v>
       </c>
       <c r="E4" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="F4" t="s">
         <v>107</v>
       </c>
       <c r="G4" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1378,7 +1384,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C5" t="s">
         <v>9</v>
@@ -1387,7 +1393,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="F5" t="s">
         <v>13</v>
@@ -1401,7 +1407,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C6" t="s">
         <v>11</v>
@@ -1410,13 +1416,13 @@
         <v>12</v>
       </c>
       <c r="E6" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="F6" t="s">
         <v>58</v>
       </c>
       <c r="G6" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1424,7 +1430,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C7" t="s">
         <v>15</v>
@@ -1433,13 +1439,13 @@
         <v>16</v>
       </c>
       <c r="E7" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="F7" t="s">
         <v>20</v>
       </c>
       <c r="G7" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1447,7 +1453,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C8" t="s">
         <v>18</v>
@@ -1456,7 +1462,7 @@
         <v>19</v>
       </c>
       <c r="E8" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="F8" t="s">
         <v>23</v>
@@ -1470,7 +1476,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C9" t="s">
         <v>21</v>
@@ -1479,13 +1485,13 @@
         <v>22</v>
       </c>
       <c r="E9" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="F9" t="s">
         <v>51</v>
       </c>
       <c r="G9" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -1493,7 +1499,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C10" t="s">
         <v>25</v>
@@ -1502,13 +1508,13 @@
         <v>26</v>
       </c>
       <c r="E10" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="F10" t="s">
         <v>52</v>
       </c>
       <c r="G10" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -1516,7 +1522,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C11" t="s">
         <v>29</v>
@@ -1525,13 +1531,13 @@
         <v>30</v>
       </c>
       <c r="E11" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="F11" t="s">
         <v>108</v>
       </c>
       <c r="G11" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -1539,7 +1545,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C12" t="s">
         <v>33</v>
@@ -1548,13 +1554,13 @@
         <v>34</v>
       </c>
       <c r="E12" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="F12" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="G12" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -1562,7 +1568,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C13" t="s">
         <v>35</v>
@@ -1571,13 +1577,13 @@
         <v>36</v>
       </c>
       <c r="E13" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="F13" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="G13" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -1585,16 +1591,16 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C14" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D14" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="E14" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="F14" s="5" t="s">
         <v>41</v>
@@ -1608,7 +1614,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C15" t="s">
         <v>39</v>
@@ -1617,7 +1623,7 @@
         <v>40</v>
       </c>
       <c r="E15" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="F15" t="s">
         <v>31</v>
@@ -1631,7 +1637,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C16" t="s">
         <v>43</v>
@@ -1640,13 +1646,13 @@
         <v>44</v>
       </c>
       <c r="E16" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="F16" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="G16" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -1654,16 +1660,16 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C17" t="s">
         <v>103</v>
       </c>
       <c r="D17" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E17" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="F17" t="s">
         <v>59</v>
@@ -1677,22 +1683,22 @@
         <v>10</v>
       </c>
       <c r="B18" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C18" t="s">
         <v>104</v>
       </c>
       <c r="D18" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="E18" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="F18" t="s">
         <v>37</v>
       </c>
       <c r="G18" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -1700,19 +1706,19 @@
         <v>11</v>
       </c>
       <c r="B19" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C19" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D19" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="E19" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="G19" t="s">
         <v>38</v>
@@ -1723,22 +1729,22 @@
         <v>12</v>
       </c>
       <c r="B20" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C20" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D20" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E20" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="F20" t="s">
         <v>56</v>
       </c>
       <c r="G20" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -1746,22 +1752,22 @@
         <v>13</v>
       </c>
       <c r="B21" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C21" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D21" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="E21" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="F21" t="s">
         <v>53</v>
       </c>
       <c r="G21" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -1769,16 +1775,16 @@
         <v>14</v>
       </c>
       <c r="C22" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D22" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E22" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="F22" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="G22" t="s">
         <v>57</v>
@@ -1795,10 +1801,10 @@
         <v>49</v>
       </c>
       <c r="E23" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G23" t="s">
         <v>45</v>
@@ -1815,10 +1821,10 @@
         <v>55</v>
       </c>
       <c r="E24" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G24" t="s">
         <v>46</v>
@@ -1829,16 +1835,16 @@
         <v>17</v>
       </c>
       <c r="C25" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="D25" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="E25" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G25" t="s">
         <v>47</v>
@@ -1849,16 +1855,16 @@
         <v>18</v>
       </c>
       <c r="C26" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D26" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="E26" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="G26" t="s">
         <v>50</v>
@@ -1872,16 +1878,16 @@
         <v>61</v>
       </c>
       <c r="D27" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="E27" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="G27" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -1895,7 +1901,7 @@
         <v>63</v>
       </c>
       <c r="E28" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="F28" t="s">
         <v>27</v>
@@ -1915,13 +1921,13 @@
         <v>65</v>
       </c>
       <c r="E29" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="G29" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -1938,7 +1944,7 @@
         <v>17</v>
       </c>
       <c r="G30" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -2016,10 +2022,10 @@
         <v>81</v>
       </c>
       <c r="C36" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D36" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -2033,7 +2039,7 @@
         <v>82</v>
       </c>
       <c r="D37" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="F37" s="7"/>
     </row>
@@ -2048,7 +2054,7 @@
         <v>83</v>
       </c>
       <c r="D38" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
@@ -2168,10 +2174,10 @@
         <v>39</v>
       </c>
       <c r="C47" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D47" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
@@ -2182,7 +2188,7 @@
         <v>95</v>
       </c>
       <c r="D48" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -2241,40 +2247,40 @@
         <v>13</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>188</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -2730,7 +2736,7 @@
     </row>
     <row r="20" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H20" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
   </sheetData>
@@ -2754,10 +2760,10 @@
   <sheetData>
     <row r="1" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>13</v>
@@ -2766,45 +2772,45 @@
         <v>17</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>145</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -2854,7 +2860,7 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -2904,7 +2910,7 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -2954,7 +2960,7 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -3004,7 +3010,7 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -3054,7 +3060,7 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -3104,7 +3110,7 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -3154,7 +3160,7 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -3204,7 +3210,7 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -3254,7 +3260,7 @@
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -3304,7 +3310,7 @@
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -3354,7 +3360,7 @@
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -3404,7 +3410,7 @@
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -3454,7 +3460,7 @@
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -3504,7 +3510,7 @@
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -3554,7 +3560,7 @@
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -3604,7 +3610,7 @@
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -3654,7 +3660,7 @@
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -3704,7 +3710,7 @@
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -3754,7 +3760,7 @@
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -3804,7 +3810,7 @@
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -3854,7 +3860,7 @@
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -3904,7 +3910,7 @@
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -3954,7 +3960,7 @@
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B25">
         <v>1</v>
@@ -4004,7 +4010,7 @@
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B26">
         <v>1</v>
@@ -4054,7 +4060,7 @@
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B27">
         <v>1</v>
@@ -4104,7 +4110,7 @@
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B28">
         <v>1</v>
@@ -4154,7 +4160,7 @@
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B29">
         <v>1</v>
@@ -4204,7 +4210,7 @@
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B30">
         <v>1</v>
@@ -4254,7 +4260,7 @@
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B31">
         <v>1</v>
@@ -4304,7 +4310,7 @@
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B32">
         <v>1</v>
@@ -4354,7 +4360,7 @@
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B33">
         <v>1</v>
@@ -4404,7 +4410,7 @@
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B34">
         <v>1</v>
@@ -4454,7 +4460,7 @@
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B35">
         <v>1</v>
@@ -4504,7 +4510,7 @@
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B36">
         <v>1</v>
@@ -4554,7 +4560,7 @@
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B37">
         <v>1</v>
@@ -4604,7 +4610,7 @@
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B38">
         <v>1</v>
@@ -4654,7 +4660,7 @@
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B39">
         <v>1</v>
@@ -4704,7 +4710,7 @@
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B40">
         <v>1</v>
@@ -4754,7 +4760,7 @@
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B41">
         <v>1</v>
@@ -4804,7 +4810,7 @@
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B42">
         <v>1</v>
@@ -4854,7 +4860,7 @@
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B43">
         <v>1</v>
@@ -4904,7 +4910,7 @@
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B44">
         <v>1</v>
@@ -4954,7 +4960,7 @@
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B45">
         <v>1</v>
@@ -5004,7 +5010,7 @@
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B46">
         <v>1</v>
@@ -5054,7 +5060,7 @@
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B47">
         <v>1</v>
@@ -5104,7 +5110,7 @@
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B48">
         <v>2</v>
@@ -5154,7 +5160,7 @@
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B49">
         <v>2</v>
@@ -5204,7 +5210,7 @@
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B50">
         <v>2</v>
@@ -5254,7 +5260,7 @@
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B51">
         <v>2</v>
@@ -5304,7 +5310,7 @@
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B52">
         <v>2</v>
@@ -5354,7 +5360,7 @@
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B53">
         <v>2</v>
@@ -5404,7 +5410,7 @@
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B54">
         <v>2</v>
@@ -5454,7 +5460,7 @@
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B55">
         <v>2</v>
@@ -5504,7 +5510,7 @@
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B56">
         <v>2</v>
@@ -5554,7 +5560,7 @@
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B57">
         <v>2</v>
@@ -5604,7 +5610,7 @@
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B58">
         <v>2</v>
@@ -5654,7 +5660,7 @@
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B59">
         <v>2</v>
@@ -5704,7 +5710,7 @@
     </row>
     <row r="60" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B60">
         <v>2</v>
@@ -5754,7 +5760,7 @@
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B61">
         <v>2</v>
@@ -5804,7 +5810,7 @@
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B62">
         <v>2</v>
@@ -5854,7 +5860,7 @@
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B63">
         <v>2</v>
@@ -5904,7 +5910,7 @@
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B64">
         <v>2</v>
@@ -5954,7 +5960,7 @@
     </row>
     <row r="65" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B65">
         <v>2</v>
@@ -6004,7 +6010,7 @@
     </row>
     <row r="66" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B66">
         <v>2</v>
@@ -6054,7 +6060,7 @@
     </row>
     <row r="67" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B67">
         <v>2</v>
@@ -6104,7 +6110,7 @@
     </row>
     <row r="68" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B68">
         <v>2</v>
@@ -6154,7 +6160,7 @@
     </row>
     <row r="69" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B69">
         <v>2</v>
@@ -6204,7 +6210,7 @@
     </row>
     <row r="70" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B70">
         <v>2</v>
@@ -6254,7 +6260,7 @@
     </row>
     <row r="71" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B71">
         <v>2</v>
@@ -6304,7 +6310,7 @@
     </row>
     <row r="72" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B72">
         <v>2</v>
@@ -6354,7 +6360,7 @@
     </row>
     <row r="73" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B73">
         <v>2</v>
@@ -6404,7 +6410,7 @@
     </row>
     <row r="74" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B74">
         <v>2</v>
@@ -6454,7 +6460,7 @@
     </row>
     <row r="75" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B75">
         <v>2</v>
@@ -6504,7 +6510,7 @@
     </row>
     <row r="76" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B76">
         <v>2</v>
@@ -6554,7 +6560,7 @@
     </row>
     <row r="77" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B77">
         <v>2</v>
@@ -6604,7 +6610,7 @@
     </row>
     <row r="78" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B78">
         <v>2</v>
@@ -6654,7 +6660,7 @@
     </row>
     <row r="79" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B79">
         <v>2</v>
@@ -6704,7 +6710,7 @@
     </row>
     <row r="80" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B80">
         <v>2</v>
@@ -6754,7 +6760,7 @@
     </row>
     <row r="81" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B81">
         <v>2</v>
@@ -6804,7 +6810,7 @@
     </row>
     <row r="82" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B82">
         <v>2</v>
@@ -6854,7 +6860,7 @@
     </row>
     <row r="83" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B83">
         <v>2</v>
@@ -6904,7 +6910,7 @@
     </row>
     <row r="84" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B84">
         <v>2</v>
@@ -6954,7 +6960,7 @@
     </row>
     <row r="85" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B85">
         <v>2</v>
@@ -7004,7 +7010,7 @@
     </row>
     <row r="86" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B86">
         <v>2</v>
@@ -7054,7 +7060,7 @@
     </row>
     <row r="87" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B87">
         <v>2</v>
@@ -7104,7 +7110,7 @@
     </row>
     <row r="88" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B88">
         <v>2</v>
@@ -7154,7 +7160,7 @@
     </row>
     <row r="89" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B89">
         <v>2</v>
@@ -7204,7 +7210,7 @@
     </row>
     <row r="90" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B90">
         <v>2</v>
@@ -7254,7 +7260,7 @@
     </row>
     <row r="91" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B91">
         <v>2</v>
@@ -7304,7 +7310,7 @@
     </row>
     <row r="92" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B92">
         <v>2</v>
@@ -7354,7 +7360,7 @@
     </row>
     <row r="93" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B93">
         <v>2</v>
@@ -7404,7 +7410,7 @@
     </row>
     <row r="94" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B94">
         <v>3</v>
@@ -7454,7 +7460,7 @@
     </row>
     <row r="95" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B95">
         <v>3</v>
@@ -7504,7 +7510,7 @@
     </row>
     <row r="96" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B96">
         <v>3</v>
@@ -7554,7 +7560,7 @@
     </row>
     <row r="97" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B97">
         <v>3</v>
@@ -7604,7 +7610,7 @@
     </row>
     <row r="98" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B98">
         <v>3</v>
@@ -7654,7 +7660,7 @@
     </row>
     <row r="99" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B99">
         <v>3</v>
@@ -7704,7 +7710,7 @@
     </row>
     <row r="100" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B100">
         <v>3</v>
@@ -7754,7 +7760,7 @@
     </row>
     <row r="101" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B101">
         <v>3</v>
@@ -7804,7 +7810,7 @@
     </row>
     <row r="102" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B102">
         <v>3</v>
@@ -7854,7 +7860,7 @@
     </row>
     <row r="103" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B103">
         <v>3</v>
@@ -7904,7 +7910,7 @@
     </row>
     <row r="104" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B104">
         <v>3</v>
@@ -7954,7 +7960,7 @@
     </row>
     <row r="105" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B105">
         <v>3</v>
@@ -8004,7 +8010,7 @@
     </row>
     <row r="106" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B106">
         <v>3</v>
@@ -8054,7 +8060,7 @@
     </row>
     <row r="107" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B107">
         <v>3</v>
@@ -8104,7 +8110,7 @@
     </row>
     <row r="108" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B108">
         <v>3</v>
@@ -8154,7 +8160,7 @@
     </row>
     <row r="109" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B109">
         <v>3</v>
@@ -8204,7 +8210,7 @@
     </row>
     <row r="110" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B110">
         <v>3</v>
@@ -8254,7 +8260,7 @@
     </row>
     <row r="111" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B111">
         <v>3</v>
@@ -8304,7 +8310,7 @@
     </row>
     <row r="112" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B112">
         <v>3</v>
@@ -8354,7 +8360,7 @@
     </row>
     <row r="113" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B113">
         <v>3</v>
@@ -8404,7 +8410,7 @@
     </row>
     <row r="114" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B114">
         <v>3</v>
@@ -8454,7 +8460,7 @@
     </row>
     <row r="115" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B115">
         <v>3</v>
@@ -8504,7 +8510,7 @@
     </row>
     <row r="116" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B116">
         <v>3</v>
@@ -8554,7 +8560,7 @@
     </row>
     <row r="117" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B117">
         <v>3</v>
@@ -8604,7 +8610,7 @@
     </row>
     <row r="118" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B118">
         <v>3</v>
@@ -8654,7 +8660,7 @@
     </row>
     <row r="119" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B119">
         <v>3</v>
@@ -8704,7 +8710,7 @@
     </row>
     <row r="120" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B120">
         <v>3</v>
@@ -8754,7 +8760,7 @@
     </row>
     <row r="121" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B121">
         <v>3</v>
@@ -8804,7 +8810,7 @@
     </row>
     <row r="122" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B122">
         <v>3</v>
@@ -8854,7 +8860,7 @@
     </row>
     <row r="123" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B123">
         <v>3</v>
@@ -8904,7 +8910,7 @@
     </row>
     <row r="124" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B124">
         <v>3</v>
@@ -8954,7 +8960,7 @@
     </row>
     <row r="125" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B125">
         <v>3</v>
@@ -9004,7 +9010,7 @@
     </row>
     <row r="126" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B126">
         <v>3</v>
@@ -9054,7 +9060,7 @@
     </row>
     <row r="127" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B127">
         <v>3</v>
@@ -9104,7 +9110,7 @@
     </row>
     <row r="128" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B128">
         <v>3</v>
@@ -9154,7 +9160,7 @@
     </row>
     <row r="129" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B129">
         <v>3</v>
@@ -9204,7 +9210,7 @@
     </row>
     <row r="130" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B130">
         <v>3</v>
@@ -9254,7 +9260,7 @@
     </row>
     <row r="131" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B131">
         <v>3</v>
@@ -9304,7 +9310,7 @@
     </row>
     <row r="132" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B132">
         <v>3</v>
@@ -9354,7 +9360,7 @@
     </row>
     <row r="133" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B133">
         <v>3</v>
@@ -9404,7 +9410,7 @@
     </row>
     <row r="134" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B134">
         <v>3</v>
@@ -9454,7 +9460,7 @@
     </row>
     <row r="135" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B135">
         <v>3</v>
@@ -9504,7 +9510,7 @@
     </row>
     <row r="136" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B136">
         <v>3</v>
@@ -9554,7 +9560,7 @@
     </row>
     <row r="137" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B137">
         <v>3</v>
@@ -9604,7 +9610,7 @@
     </row>
     <row r="138" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B138">
         <v>3</v>
@@ -9654,7 +9660,7 @@
     </row>
     <row r="139" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B139">
         <v>3</v>
@@ -9727,37 +9733,37 @@
         <v>13</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>145</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -9818,37 +9824,37 @@
         <v>13</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>145</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -9912,37 +9918,37 @@
         <v>17</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>145</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -10009,37 +10015,37 @@
         <v>17</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>145</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -10103,10 +10109,10 @@
         <v>13</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -10140,7 +10146,7 @@
         <v>102</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -10153,7 +10159,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -10260,16 +10266,16 @@
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>260</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>262</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -10855,40 +10861,40 @@
         <v>17</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>145</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -14948,7 +14954,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
@@ -14962,7 +14968,7 @@
         <v>102</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -15063,7 +15069,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B14" s="11">
         <v>1</v>
@@ -15103,7 +15109,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B19" s="11">
         <v>0</v>
@@ -15111,15 +15117,15 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B21" s="11">
         <v>0</v>
@@ -15142,31 +15148,31 @@
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>191</v>
+      </c>
+      <c r="B1" t="s">
+        <v>192</v>
+      </c>
+      <c r="C1" t="s">
         <v>193</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>194</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>195</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>196</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
+        <v>115</v>
+      </c>
+      <c r="H1" t="s">
+        <v>122</v>
+      </c>
+      <c r="I1" t="s">
         <v>197</v>
-      </c>
-      <c r="F1" t="s">
-        <v>198</v>
-      </c>
-      <c r="G1" t="s">
-        <v>117</v>
-      </c>
-      <c r="H1" t="s">
-        <v>124</v>
-      </c>
-      <c r="I1" t="s">
-        <v>199</v>
       </c>
     </row>
   </sheetData>
@@ -15176,36 +15182,105 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C27"/>
+  <dimension ref="A1:AA6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="16.28515625" customWidth="1"/>
-    <col min="26" max="26" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.28515625" customWidth="1"/>
+    <col min="22" max="22" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B1" t="s">
-        <v>256</v>
-      </c>
-      <c r="C1" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="B1" s="1" t="s">
         <v>106</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>254</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -15213,10 +15288,70 @@
       <c r="C2">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>107</v>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>2</v>
+      </c>
+      <c r="G2">
+        <v>10</v>
+      </c>
+      <c r="H2">
+        <v>0.5</v>
+      </c>
+      <c r="I2">
+        <v>0.4</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>1</v>
+      </c>
+      <c r="N2">
+        <v>1</v>
+      </c>
+      <c r="O2">
+        <v>1</v>
+      </c>
+      <c r="P2">
+        <v>1</v>
+      </c>
+      <c r="Q2">
+        <v>1</v>
+      </c>
+      <c r="R2">
+        <v>1</v>
+      </c>
+      <c r="S2">
+        <v>1</v>
+      </c>
+      <c r="T2">
+        <v>0</v>
+      </c>
+      <c r="U2">
+        <v>0</v>
+      </c>
+      <c r="V2">
+        <v>0</v>
+      </c>
+      <c r="X2">
+        <v>0</v>
+      </c>
+      <c r="Z2">
+        <v>0</v>
+      </c>
+      <c r="AA2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>263</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -15224,220 +15359,47 @@
       <c r="C3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5">
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6">
+      <c r="F3">
         <v>2</v>
       </c>
-      <c r="C6">
+      <c r="G3">
+        <v>10</v>
+      </c>
+      <c r="H3">
+        <v>0.94599999999999995</v>
+      </c>
+      <c r="I3">
+        <v>10.3</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>1</v>
+      </c>
+      <c r="N3">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B7">
-        <v>10</v>
-      </c>
-      <c r="C7">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B8">
-        <v>0.5</v>
-      </c>
-      <c r="C8">
-        <v>0.94599999999999995</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B9">
-        <v>0.4</v>
-      </c>
-      <c r="C9">
-        <v>10.3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="B13">
-        <v>1</v>
-      </c>
-      <c r="C13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B14">
-        <v>1</v>
-      </c>
-      <c r="C14">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="B15">
-        <v>1</v>
-      </c>
-      <c r="C15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="B18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="B21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="B22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="B24">
-        <v>0</v>
-      </c>
-      <c r="C24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="B26">
-        <v>0</v>
-      </c>
-      <c r="C26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="B27">
-        <v>1</v>
-      </c>
-      <c r="C27">
-        <v>1</v>
-      </c>
-    </row>
+      <c r="O3">
+        <v>1</v>
+      </c>
+      <c r="X3">
+        <v>0</v>
+      </c>
+      <c r="Z3">
+        <v>0</v>
+      </c>
+      <c r="AA3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -15464,27 +15426,27 @@
         <v>13</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>121</v>
-      </c>
       <c r="I1" s="1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -15513,7 +15475,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -15542,7 +15504,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -15571,7 +15533,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -15600,7 +15562,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -15629,7 +15591,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -15658,7 +15620,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -15687,7 +15649,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -15716,7 +15678,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -15745,7 +15707,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -15774,7 +15736,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -15803,7 +15765,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -15832,7 +15794,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -15868,8 +15830,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:H47"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="J55" sqref="J55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15890,24 +15852,24 @@
         <v>13</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>119</v>
-      </c>
       <c r="G1" s="8" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B2">
         <v>2</v>
@@ -15933,7 +15895,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -15959,7 +15921,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B4">
         <v>2</v>
@@ -15985,7 +15947,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B5">
         <v>2</v>
@@ -16011,7 +15973,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B6">
         <v>2</v>
@@ -16037,7 +15999,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B7">
         <v>2</v>
@@ -16063,7 +16025,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B8">
         <v>2</v>
@@ -16089,7 +16051,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B9">
         <v>2</v>
@@ -16115,7 +16077,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B10">
         <v>2</v>
@@ -16141,7 +16103,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B11">
         <v>2</v>
@@ -16167,7 +16129,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B12">
         <v>2</v>
@@ -16193,7 +16155,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B13">
         <v>2</v>
@@ -16219,7 +16181,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B14">
         <v>2</v>
@@ -16245,7 +16207,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B15">
         <v>2</v>
@@ -16271,7 +16233,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B16">
         <v>2</v>
@@ -16297,7 +16259,7 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B17">
         <v>2</v>
@@ -16323,7 +16285,7 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B18">
         <v>2</v>
@@ -16349,7 +16311,7 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B19">
         <v>2</v>
@@ -16375,7 +16337,7 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B20">
         <v>2</v>
@@ -16401,7 +16363,7 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B21">
         <v>2</v>
@@ -16427,7 +16389,7 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B22">
         <v>2</v>
@@ -16453,7 +16415,7 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B23">
         <v>2</v>
@@ -16479,7 +16441,7 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B24">
         <v>2</v>
@@ -16505,7 +16467,7 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B25">
         <v>2</v>
@@ -16531,7 +16493,7 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B26">
         <v>2</v>
@@ -16557,7 +16519,7 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B27">
         <v>2</v>
@@ -16583,7 +16545,7 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B28">
         <v>2</v>
@@ -16609,7 +16571,7 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B29">
         <v>2</v>
@@ -16635,7 +16597,7 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B30">
         <v>2</v>
@@ -16661,7 +16623,7 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B31">
         <v>2</v>
@@ -16687,7 +16649,7 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B32">
         <v>2</v>
@@ -16713,7 +16675,7 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B33">
         <v>2</v>
@@ -16739,7 +16701,7 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B34">
         <v>2</v>
@@ -16765,7 +16727,7 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B35">
         <v>2</v>
@@ -16791,7 +16753,7 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B36">
         <v>2</v>
@@ -16817,7 +16779,7 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B37">
         <v>2</v>
@@ -16843,7 +16805,7 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B38">
         <v>2</v>
@@ -16869,7 +16831,7 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B39">
         <v>2</v>
@@ -16895,7 +16857,7 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B40">
         <v>2</v>
@@ -16921,7 +16883,7 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B41">
         <v>2</v>
@@ -16947,7 +16909,7 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B42">
         <v>2</v>
@@ -16973,7 +16935,7 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B43">
         <v>2</v>
@@ -16999,7 +16961,7 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B44">
         <v>2</v>
@@ -17025,7 +16987,7 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B45">
         <v>2</v>
@@ -17051,7 +17013,7 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B46">
         <v>2</v>
@@ -17077,7 +17039,7 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B47">
         <v>2</v>
@@ -17135,54 +17097,54 @@
         <v>17</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>133</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="2" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -17241,7 +17203,7 @@
     </row>
     <row r="3" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -17302,7 +17264,7 @@
     </row>
     <row r="4" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -17361,7 +17323,7 @@
     </row>
     <row r="5" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -17420,7 +17382,7 @@
     </row>
     <row r="6" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -17482,7 +17444,7 @@
     </row>
     <row r="7" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -17541,7 +17503,7 @@
     </row>
     <row r="8" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -17600,7 +17562,7 @@
     </row>
     <row r="9" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -17660,7 +17622,7 @@
     </row>
     <row r="10" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -17720,7 +17682,7 @@
     </row>
     <row r="11" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -17781,7 +17743,7 @@
     </row>
     <row r="12" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -17841,7 +17803,7 @@
     </row>
     <row r="13" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -17901,7 +17863,7 @@
     </row>
     <row r="14" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B14">
         <v>2</v>
@@ -17963,7 +17925,7 @@
     </row>
     <row r="15" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B15">
         <v>2</v>
@@ -18026,7 +17988,7 @@
     </row>
     <row r="16" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B16">
         <v>2</v>
@@ -18087,7 +18049,7 @@
     </row>
     <row r="17" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B17">
         <v>2</v>
@@ -18146,7 +18108,7 @@
     </row>
     <row r="18" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B18">
         <v>2</v>
@@ -18206,7 +18168,7 @@
     </row>
     <row r="19" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B19">
         <v>2</v>
@@ -18265,7 +18227,7 @@
     </row>
     <row r="20" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B20">
         <v>2</v>
@@ -18324,7 +18286,7 @@
     </row>
     <row r="21" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B21">
         <v>2</v>
@@ -18383,7 +18345,7 @@
     </row>
     <row r="22" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B22">
         <v>2</v>
@@ -18442,7 +18404,7 @@
     </row>
     <row r="23" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B23">
         <v>2</v>
@@ -18501,7 +18463,7 @@
     </row>
     <row r="24" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B24">
         <v>2</v>
@@ -18560,7 +18522,7 @@
     </row>
     <row r="25" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B25">
         <v>2</v>
@@ -18619,7 +18581,7 @@
     </row>
     <row r="26" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B26">
         <v>2</v>
@@ -18678,7 +18640,7 @@
     </row>
     <row r="27" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B27">
         <v>2</v>
@@ -18737,7 +18699,7 @@
     </row>
     <row r="28" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B28">
         <v>2</v>
@@ -18796,7 +18758,7 @@
     </row>
     <row r="29" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B29">
         <v>2</v>
@@ -18855,7 +18817,7 @@
     </row>
     <row r="30" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B30">
         <v>2</v>
@@ -18914,7 +18876,7 @@
     </row>
     <row r="31" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B31">
         <v>2</v>
@@ -18973,7 +18935,7 @@
     </row>
     <row r="32" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B32">
         <v>2</v>
@@ -19032,7 +18994,7 @@
     </row>
     <row r="33" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B33">
         <v>2</v>
@@ -19091,7 +19053,7 @@
     </row>
     <row r="34" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B34">
         <v>2</v>
@@ -19150,7 +19112,7 @@
     </row>
     <row r="35" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B35">
         <v>2</v>
@@ -19209,7 +19171,7 @@
     </row>
     <row r="36" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B36">
         <v>2</v>
@@ -19268,7 +19230,7 @@
     </row>
     <row r="37" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B37">
         <v>2</v>
@@ -19327,7 +19289,7 @@
     </row>
     <row r="38" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B38">
         <v>2</v>
@@ -19386,7 +19348,7 @@
     </row>
     <row r="39" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B39">
         <v>2</v>
@@ -19445,7 +19407,7 @@
     </row>
     <row r="40" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B40">
         <v>2</v>
@@ -19504,7 +19466,7 @@
     </row>
     <row r="41" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B41">
         <v>2</v>
@@ -19563,7 +19525,7 @@
     </row>
     <row r="42" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B42">
         <v>2</v>
@@ -19622,7 +19584,7 @@
     </row>
     <row r="43" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B43">
         <v>2</v>
@@ -19681,7 +19643,7 @@
     </row>
     <row r="44" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B44">
         <v>2</v>
@@ -19740,7 +19702,7 @@
     </row>
     <row r="45" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B45">
         <v>2</v>
@@ -19799,7 +19761,7 @@
     </row>
     <row r="46" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B46">
         <v>2</v>
@@ -19859,7 +19821,7 @@
     </row>
     <row r="47" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B47">
         <v>2</v>
@@ -19918,7 +19880,7 @@
     </row>
     <row r="48" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B48">
         <v>2</v>
@@ -19977,7 +19939,7 @@
     </row>
     <row r="49" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B49">
         <v>2</v>
@@ -20036,7 +19998,7 @@
     </row>
     <row r="50" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B50">
         <v>2</v>
@@ -20095,7 +20057,7 @@
     </row>
     <row r="51" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B51">
         <v>2</v>
@@ -20154,7 +20116,7 @@
     </row>
     <row r="52" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B52">
         <v>2</v>
@@ -20213,7 +20175,7 @@
     </row>
     <row r="53" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B53">
         <v>2</v>
@@ -20272,7 +20234,7 @@
     </row>
     <row r="54" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B54">
         <v>2</v>
@@ -20331,7 +20293,7 @@
     </row>
     <row r="55" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B55">
         <v>2</v>
@@ -20390,7 +20352,7 @@
     </row>
     <row r="56" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B56">
         <v>2</v>
@@ -20449,7 +20411,7 @@
     </row>
     <row r="57" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B57">
         <v>2</v>
@@ -20542,40 +20504,40 @@
         <v>17</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>133</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="2" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -20952,7 +20914,7 @@
   <sheetData>
     <row r="1" spans="1:34" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>13</v>
@@ -20961,102 +20923,102 @@
         <v>17</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="X1" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="Y1" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="Z1" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="AA1" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>164</v>
-      </c>
-      <c r="AG1" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="AH1" s="1" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="2" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -21103,7 +21065,7 @@
     </row>
     <row r="3" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -21151,7 +21113,7 @@
     </row>
     <row r="4" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -21199,7 +21161,7 @@
     </row>
     <row r="5" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -21247,7 +21209,7 @@
     </row>
     <row r="6" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -21295,7 +21257,7 @@
     </row>
     <row r="7" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -21343,7 +21305,7 @@
     </row>
     <row r="8" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -21391,7 +21353,7 @@
     </row>
     <row r="9" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -21439,7 +21401,7 @@
     </row>
     <row r="10" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -21487,7 +21449,7 @@
     </row>
     <row r="11" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -21535,7 +21497,7 @@
     </row>
     <row r="12" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -21583,7 +21545,7 @@
     </row>
     <row r="13" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -21631,7 +21593,7 @@
     </row>
     <row r="14" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -21679,7 +21641,7 @@
     </row>
     <row r="15" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -21727,7 +21689,7 @@
     </row>
     <row r="16" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -21775,7 +21737,7 @@
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -21823,7 +21785,7 @@
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -21871,7 +21833,7 @@
     </row>
     <row r="19" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -21919,7 +21881,7 @@
     </row>
     <row r="20" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -21967,7 +21929,7 @@
     </row>
     <row r="21" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -22015,7 +21977,7 @@
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -22063,7 +22025,7 @@
     </row>
     <row r="23" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -22111,7 +22073,7 @@
     </row>
     <row r="24" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -22159,7 +22121,7 @@
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B25">
         <v>1</v>
@@ -22207,7 +22169,7 @@
     </row>
     <row r="26" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B26">
         <v>1</v>
@@ -22255,7 +22217,7 @@
     </row>
     <row r="27" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B27">
         <v>1</v>
@@ -22303,7 +22265,7 @@
     </row>
     <row r="28" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B28">
         <v>1</v>
@@ -22351,7 +22313,7 @@
     </row>
     <row r="29" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B29">
         <v>1</v>
@@ -22399,7 +22361,7 @@
     </row>
     <row r="30" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B30">
         <v>1</v>
@@ -22447,7 +22409,7 @@
     </row>
     <row r="31" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B31">
         <v>1</v>
@@ -22495,7 +22457,7 @@
     </row>
     <row r="32" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B32">
         <v>1</v>
@@ -22543,7 +22505,7 @@
     </row>
     <row r="33" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B33">
         <v>1</v>
@@ -22591,7 +22553,7 @@
     </row>
     <row r="34" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B34">
         <v>1</v>
@@ -22639,7 +22601,7 @@
     </row>
     <row r="35" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B35">
         <v>1</v>
@@ -22687,7 +22649,7 @@
     </row>
     <row r="36" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B36">
         <v>1</v>
@@ -22735,7 +22697,7 @@
     </row>
     <row r="37" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B37">
         <v>1</v>
@@ -22783,7 +22745,7 @@
     </row>
     <row r="38" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B38">
         <v>1</v>
@@ -22831,7 +22793,7 @@
     </row>
     <row r="39" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B39">
         <v>1</v>
@@ -22879,7 +22841,7 @@
     </row>
     <row r="40" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B40">
         <v>1</v>
@@ -22927,7 +22889,7 @@
     </row>
     <row r="41" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B41">
         <v>1</v>
@@ -22975,7 +22937,7 @@
     </row>
     <row r="42" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B42">
         <v>1</v>
@@ -23023,7 +22985,7 @@
     </row>
     <row r="43" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B43">
         <v>1</v>
@@ -23071,7 +23033,7 @@
     </row>
     <row r="44" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B44">
         <v>1</v>
@@ -23119,7 +23081,7 @@
     </row>
     <row r="45" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B45">
         <v>1</v>
@@ -23167,7 +23129,7 @@
     </row>
     <row r="46" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B46">
         <v>1</v>
@@ -23215,7 +23177,7 @@
     </row>
     <row r="47" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B47">
         <v>1</v>
@@ -23425,10 +23387,10 @@
   <sheetData>
     <row r="1" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>13</v>
@@ -23437,45 +23399,45 @@
         <v>17</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>176</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -23525,7 +23487,7 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -23575,7 +23537,7 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -23625,7 +23587,7 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -23675,7 +23637,7 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -23725,7 +23687,7 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -23775,7 +23737,7 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -23825,7 +23787,7 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -23875,7 +23837,7 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -23925,7 +23887,7 @@
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -23975,7 +23937,7 @@
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B12">
         <v>1</v>

</xml_diff>